<commit_message>
inserindo tela de atuação user
</commit_message>
<xml_diff>
--- a/db/controle_estoque.xlsx
+++ b/db/controle_estoque.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1912,15 +1912,83 @@
     <row r="33">
       <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr"/>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>hoje</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>nome</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>produto</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>-6</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>puta</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>quatro</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>naotem</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>naotem</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
corrigindo query diferença user - admin
</commit_message>
<xml_diff>
--- a/db/controle_estoque.xlsx
+++ b/db/controle_estoque.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1989,6 +1989,318 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>01/03/2025</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>01/03/2025</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>01/03/2025</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>01/03/2025</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>01/03/2025</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
tela de edição funcional
</commit_message>
<xml_diff>
--- a/db/controle_estoque.xlsx
+++ b/db/controle_estoque.xlsx
@@ -1992,52 +1992,52 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>01/03/2025</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
+      <c r="H35" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr">
+      <c r="I35" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>89</t>
         </is>
       </c>
     </row>
@@ -2054,42 +2054,42 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>89</t>
+          <t>admin</t>
         </is>
       </c>
     </row>
@@ -2101,22 +2101,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2126,17 +2126,17 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2153,22 +2153,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2178,22 +2178,22 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>admin</t>
+          <t>user</t>
         </is>
       </c>
     </row>
@@ -2205,22 +2205,22 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2230,17 +2230,17 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -2252,7 +2252,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>01/03/2025</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2262,42 +2262,42 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8749</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>49684</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>40935</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>user</t>
+          <t>9</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
corrigindo matematica do total
</commit_message>
<xml_diff>
--- a/db/controle_estoque.xlsx
+++ b/db/controle_estoque.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1115,22 +1115,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>eli</t>
+          <t>renan</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>coca</t>
+          <t>coxinha</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>-50</v>
+        <v>-10</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1147,53 +1147,263 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>nao tem</t>
+          <t>352456</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
+        <v>45769</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>coca</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>20</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-20</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>aluno</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>quarto</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>25</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>45769</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>coca</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>20</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-20</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>aluno</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>quarto</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>25</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>45769</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>coca</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>10</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-10</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>aluno</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>terceiro</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>68765</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>45769</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>coca</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-10</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>aluno</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>quarto</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>25</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45769</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>pedro</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>coca</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>10</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-10</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>aluno</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>quarto</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>25</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
         <v>45773</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>renan</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>coxinha</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>eli</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>coca</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="inlineStr">
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="inlineStr">
         <is>
           <t>-10</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>aluno</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>terceiro</t>
         </is>
       </c>
-      <c r="I19" t="n">
+      <c r="I24" t="n">
         <v>654</v>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>352456</t>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>nao tem</t>
         </is>
       </c>
     </row>

</xml_diff>